<commit_message>
Set up Class: Unit, Skill
</commit_message>
<xml_diff>
--- a/skilldata.xlsx
+++ b/skilldata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu.zehu\Documents\SIFIWARCHESS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97F1A99-46E7-4D4D-879B-872E1B482A01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16284C9-012C-448F-921D-D16397383461}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -88,6 +88,36 @@
   </si>
   <si>
     <t>Shocking</t>
+  </si>
+  <si>
+    <t>tar_type</t>
+  </si>
+  <si>
+    <t>damage</t>
+  </si>
+  <si>
+    <t>cold_t</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>shield</t>
+  </si>
+  <si>
+    <t>uhp</t>
+  </si>
+  <si>
+    <t>mana</t>
+  </si>
+  <si>
+    <t>armor</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>range</t>
   </si>
 </sst>
 </file>
@@ -419,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G10"/>
+  <dimension ref="A2:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -430,126 +460,183 @@
     <col min="1" max="1" width="14.73046875" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.1328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.3984375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="9.06640625" style="1"/>
-    <col min="6" max="6" width="20.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.86328125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.06640625" style="1"/>
+    <col min="4" max="7" width="9.06640625" style="1"/>
+    <col min="8" max="8" width="20.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.86328125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C5" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C5" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D5" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C9" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D6" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="D9" s="1">
         <v>-1</v>
       </c>
-      <c r="E9" s="1">
+      <c r="H9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D13" s="1">
         <v>1</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="1">
+      <c r="I13" s="1">
         <v>-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test Switch Logic; Continuous Logic with bugs
</commit_message>
<xml_diff>
--- a/skilldata.xlsx
+++ b/skilldata.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu.zehu\Documents\SIFIWARCHESS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA393E10-55BE-4F1D-B5DA-8CDE426135DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4ADA18-3491-49D6-ABD9-E1D0C656A2A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -118,6 +127,21 @@
   </si>
   <si>
     <t>uph</t>
+  </si>
+  <si>
+    <t>Adrenaline</t>
+  </si>
+  <si>
+    <t>self</t>
+  </si>
+  <si>
+    <t>uhp/speed/freq</t>
+  </si>
+  <si>
+    <t>-20/1/2</t>
+  </si>
+  <si>
+    <t>=F17</t>
   </si>
 </sst>
 </file>
@@ -161,12 +185,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -449,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I13"/>
+  <dimension ref="A2:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -462,7 +492,7 @@
     <col min="3" max="3" width="10.3984375" style="1" customWidth="1"/>
     <col min="4" max="7" width="9.06640625" style="1"/>
     <col min="8" max="8" width="20.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.86328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.86328125" style="3" customWidth="1"/>
     <col min="10" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
@@ -578,7 +608,7 @@
       <c r="H11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -596,7 +626,7 @@
         <v>-1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -607,40 +637,134 @@
       <c r="H12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
       </c>
       <c r="G13" s="1">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="1">
         <v>0</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I14" s="3">
         <v>-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Medical logic - without test
</commit_message>
<xml_diff>
--- a/skilldata.xlsx
+++ b/skilldata.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu.zehu\Documents\SIFIWARCHESS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4DC1DB-71DD-42BC-AD88-4EFAD88AD9D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C99DE46-5C6A-4125-B3B4-49C37C80FF02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>name</t>
   </si>
@@ -51,9 +51,6 @@
     <t>continuous</t>
   </si>
   <si>
-    <t>onetime</t>
-  </si>
-  <si>
     <t>manacost</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>uhp/speed</t>
   </si>
   <si>
-    <t>10/-1</t>
-  </si>
-  <si>
     <t>Shield Defense</t>
   </si>
   <si>
@@ -135,10 +129,61 @@
     <t>uhp/speed/freq</t>
   </si>
   <si>
-    <t>-20/1/2</t>
-  </si>
-  <si>
     <t>uhp</t>
+  </si>
+  <si>
+    <t>clearup</t>
+  </si>
+  <si>
+    <t>backlash</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>20/-1</t>
+  </si>
+  <si>
+    <t>-30/1/2</t>
+  </si>
+  <si>
+    <t>Medican</t>
+  </si>
+  <si>
+    <t>Medical nanoworm</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>g_b</t>
+  </si>
+  <si>
+    <t>Emergency</t>
+  </si>
+  <si>
+    <t>medical</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Siege mode</t>
+  </si>
+  <si>
+    <t>damage/speed/freq/range</t>
+  </si>
+  <si>
+    <t>Siege Tank</t>
+  </si>
+  <si>
+    <t>330/-4/-4/4</t>
   </si>
 </sst>
 </file>
@@ -162,15 +207,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -178,22 +229,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -202,6 +280,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -476,300 +559,348 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J26"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.73046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" style="1" customWidth="1"/>
-    <col min="4" max="7" width="9.06640625" style="1"/>
-    <col min="8" max="8" width="20.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.86328125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="14.73046875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.1328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.3984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.06640625" style="4"/>
+    <col min="5" max="5" width="9.06640625" style="2"/>
+    <col min="6" max="6" width="9.06640625" style="7"/>
+    <col min="7" max="7" width="9.06640625" style="4"/>
+    <col min="8" max="8" width="25.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="24.86328125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.06640625" style="4"/>
+    <col min="11" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="H2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="H3" s="1" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C4" s="1" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>4</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="2">
+        <v>-2</v>
+      </c>
+      <c r="J14" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="7">
+        <v>50</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="1">
+      <c r="I15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="7">
+        <v>100</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="4">
         <v>-1</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C5" s="1" t="s">
+      <c r="E17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
         <v>3</v>
       </c>
-      <c r="D5" s="1">
-        <v>-1</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1">
-        <v>-1</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="1">
-        <v>-1</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="1">
-        <v>2</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>4</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="3">
-        <v>-2</v>
-      </c>
-      <c r="J14" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>33</v>
+      <c r="H17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Skill target type logic
</commit_message>
<xml_diff>
--- a/skilldata.xlsx
+++ b/skilldata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu.zehu\Documents\SIFIWARCHESS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C99DE46-5C6A-4125-B3B4-49C37C80FF02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E2135C-B05F-4599-92B9-C39EB9850355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
   <si>
     <t>name</t>
   </si>
@@ -177,13 +177,55 @@
     <t>Siege mode</t>
   </si>
   <si>
-    <t>damage/speed/freq/range</t>
-  </si>
-  <si>
     <t>Siege Tank</t>
   </si>
   <si>
-    <t>330/-4/-4/4</t>
+    <t>l/h/speed/freq/range</t>
+  </si>
+  <si>
+    <t>310/330/-4/-4/4</t>
+  </si>
+  <si>
+    <t>EMP</t>
+  </si>
+  <si>
+    <t>Storm Chariot</t>
+  </si>
+  <si>
+    <t>shield/speed</t>
+  </si>
+  <si>
+    <t>-50/2</t>
+  </si>
+  <si>
+    <t>Piercing missile</t>
+  </si>
+  <si>
+    <t>g_m</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>Frigate</t>
+  </si>
+  <si>
+    <t>Battleship</t>
+  </si>
+  <si>
+    <t>Space jump</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>g/a/g_freq/a_freq</t>
+  </si>
+  <si>
+    <t>550/180/-14/-34</t>
+  </si>
+  <si>
+    <t>Volley</t>
   </si>
 </sst>
 </file>
@@ -559,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -570,10 +612,10 @@
     <col min="1" max="1" width="14.73046875" style="2" customWidth="1"/>
     <col min="2" max="2" width="18.1328125" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.3984375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.06640625" style="4"/>
-    <col min="5" max="5" width="9.06640625" style="2"/>
-    <col min="6" max="6" width="9.06640625" style="7"/>
-    <col min="7" max="7" width="9.06640625" style="4"/>
+    <col min="4" max="4" width="5.59765625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="7.59765625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.265625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="6.3984375" style="4" customWidth="1"/>
     <col min="8" max="8" width="25.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="24.86328125" style="2" customWidth="1"/>
     <col min="10" max="10" width="9.06640625" style="4"/>
@@ -873,33 +915,161 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="7">
+        <v>75</v>
+      </c>
+      <c r="G17" s="4">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>3</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="I18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
         <v>3</v>
       </c>
-      <c r="D17" s="4">
-        <v>-1</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="H19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="7">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4">
-        <v>3</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J17" s="4">
+      <c r="F20" s="7">
+        <v>150</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="7">
+        <v>100</v>
+      </c>
+      <c r="G21" s="4">
+        <v>4</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J21" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Get Unit and skill from DB; prepare for tests
</commit_message>
<xml_diff>
--- a/skilldata.xlsx
+++ b/skilldata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu.zehu\Documents\SIFIWARCHESS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFA4A8E-8AD5-43D4-95DC-7E95537D9B40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C4D99F-8871-4F9A-BC9F-F3B1CF71D03C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
   <si>
     <t>name</t>
   </si>
@@ -216,23 +216,29 @@
     <t>Space jump</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>g/a/g_freq/a_freq</t>
   </si>
   <si>
-    <t>550/180/-14/-34</t>
-  </si>
-  <si>
     <t>Volley</t>
+  </si>
+  <si>
+    <t>720/345/-28/-72</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>aoe</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +250,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -601,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -622,7 +634,7 @@
     <col min="11" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
@@ -630,7 +642,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
@@ -641,7 +653,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C3" s="2" t="s">
         <v>43</v>
       </c>
@@ -652,7 +664,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C4" s="2" t="s">
         <v>32</v>
       </c>
@@ -663,7 +675,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C5" s="2" t="s">
         <v>33</v>
       </c>
@@ -674,7 +686,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
@@ -685,7 +697,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
@@ -696,7 +708,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
@@ -707,7 +719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
@@ -718,7 +730,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>0</v>
       </c>
@@ -749,8 +761,11 @@
       <c r="J11" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K11" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -781,8 +796,11 @@
       <c r="J12" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K12" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -813,8 +831,11 @@
       <c r="J13" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -845,8 +866,11 @@
       <c r="J14" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K14" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -877,8 +901,11 @@
       <c r="J15" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K15" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
@@ -909,8 +936,11 @@
       <c r="J16" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K16" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>51</v>
       </c>
@@ -941,8 +971,11 @@
       <c r="J17" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K17" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -973,8 +1006,11 @@
       <c r="J18" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K18" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
@@ -1005,8 +1041,11 @@
       <c r="J19" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K19" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -1032,18 +1071,21 @@
         <v>13</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J20" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K20" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>4</v>
@@ -1061,7 +1103,7 @@
         <v>4</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>62</v>
@@ -1069,8 +1111,12 @@
       <c r="J21" s="4">
         <v>0</v>
       </c>
+      <c r="K21" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Test Marine's skills; Teat Attack Trigger
</commit_message>
<xml_diff>
--- a/skilldata.xlsx
+++ b/skilldata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu.zehu\Documents\SIFIWARCHESS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C4D99F-8871-4F9A-BC9F-F3B1CF71D03C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69181AD-7D85-475F-B324-E5BD2F699A22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="74">
   <si>
     <t>name</t>
   </si>
@@ -180,12 +180,6 @@
     <t>Siege Tank</t>
   </si>
   <si>
-    <t>l/h/speed/freq/range</t>
-  </si>
-  <si>
-    <t>310/330/-4/-4/4</t>
-  </si>
-  <si>
     <t>EMP</t>
   </si>
   <si>
@@ -195,9 +189,6 @@
     <t>shield/speed</t>
   </si>
   <si>
-    <t>-50/2</t>
-  </si>
-  <si>
     <t>Piercing missile</t>
   </si>
   <si>
@@ -232,6 +223,39 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>-50/-2</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>l/h/speed/g_freq/range/g_aoe</t>
+  </si>
+  <si>
+    <t>310/330/-4/-4/4/1</t>
   </si>
 </sst>
 </file>
@@ -613,505 +637,539 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.73046875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.1328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="5.59765625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="7.59765625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.265625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="6.3984375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="24.86328125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.06640625" style="4"/>
-    <col min="11" max="16384" width="9.06640625" style="2"/>
+    <col min="1" max="1" width="9.06640625" style="4"/>
+    <col min="2" max="2" width="14.73046875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.1328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.3984375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="5.59765625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="7.59765625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.265625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="6.3984375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="24.86328125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.06640625" style="4"/>
+    <col min="12" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C2" s="2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C4" s="2" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C5" s="2" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C6" s="2" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C7" s="2" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C8" s="2" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C9" s="2" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="5" t="s">
-        <v>0</v>
+    <row r="11" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="H11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="K11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
+      <c r="L11" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E12" s="4">
         <v>-1</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="7">
-        <v>0</v>
-      </c>
-      <c r="G12" s="4">
+      <c r="G12" s="7">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
         <v>1</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="4">
-        <v>0</v>
-      </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="4">
+      <c r="E13" s="4">
         <v>2</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="7">
-        <v>0</v>
-      </c>
-      <c r="G13" s="4">
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
         <v>4</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J13" s="4">
-        <v>0</v>
-      </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="4">
+      <c r="E14" s="4">
         <v>1</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="7">
-        <v>0</v>
-      </c>
-      <c r="G14" s="4">
+      <c r="G14" s="7">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
         <v>1</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>-2</v>
       </c>
-      <c r="J14" s="4">
+      <c r="K14" s="4">
         <v>5</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="4">
+      <c r="E15" s="4">
         <v>2</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="7">
+      <c r="G15" s="7">
         <v>50</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="4">
+      <c r="K15" s="4">
         <v>4</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="4">
+      <c r="E16" s="4">
         <v>1</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="7">
+      <c r="G16" s="7">
         <v>100</v>
       </c>
-      <c r="G16" s="4">
+      <c r="H16" s="4">
         <v>1</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J16" s="4">
+      <c r="K16" s="4">
         <v>4</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="7">
+        <v>75</v>
+      </c>
+      <c r="H17" s="4">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K17" s="4">
+        <v>6</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="7">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>3</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="D19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="7">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>3</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K19" s="4">
+        <v>8</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="4">
+      <c r="E20" s="4">
         <v>1</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="7">
-        <v>75</v>
-      </c>
-      <c r="G17" s="4">
+      <c r="F20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="7">
+        <v>150</v>
+      </c>
+      <c r="H20" s="4">
         <v>1</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J17" s="4">
-        <v>6</v>
-      </c>
-      <c r="K17" s="2" t="s">
+      <c r="I20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="4">
-        <v>-1</v>
-      </c>
-      <c r="E18" s="2" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="7">
-        <v>0</v>
-      </c>
-      <c r="G18" s="4">
-        <v>3</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J18" s="4">
-        <v>0</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A19" s="1" t="s">
+      <c r="G21" s="7">
+        <v>100</v>
+      </c>
+      <c r="H21" s="4">
+        <v>4</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="7">
-        <v>0</v>
-      </c>
-      <c r="G19" s="4">
-        <v>3</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J19" s="4">
-        <v>8</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="4">
-        <v>1</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="7">
-        <v>150</v>
-      </c>
-      <c r="G20" s="4">
-        <v>1</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J20" s="4">
-        <v>0</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="7">
-        <v>100</v>
-      </c>
-      <c r="G21" s="4">
-        <v>4</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J21" s="4">
-        <v>0</v>
-      </c>
-      <c r="K21" s="2" t="s">
+      <c r="K21" s="4">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjust some continuous skills' period
</commit_message>
<xml_diff>
--- a/skilldata.xlsx
+++ b/skilldata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu.zehu\Documents\SIFIWARCHESS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69181AD-7D85-475F-B324-E5BD2F699A22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4299BDD9-FA82-485D-838D-E4AB052B2A8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -640,7 +640,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -883,7 +883,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>10</v>
@@ -997,7 +997,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>10</v>
@@ -1006,7 +1006,7 @@
         <v>75</v>
       </c>
       <c r="H17" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
User specific Create and Read Ops for Project Tasks
</commit_message>
<xml_diff>
--- a/skilldata.xlsx
+++ b/skilldata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu.zehu\Documents\SIFIWARCHESS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1796EAD-09A9-4E6E-82BA-8613421F9BA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF59C4C2-9277-4A7F-B71F-5E02029670FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="85">
   <si>
     <t>name</t>
   </si>
@@ -265,6 +265,30 @@
   </si>
   <si>
     <t>75</t>
+  </si>
+  <si>
+    <t>Assault spikes</t>
+  </si>
+  <si>
+    <t>Bettle</t>
+  </si>
+  <si>
+    <t>armor/damage/range</t>
+  </si>
+  <si>
+    <t>2/4/-2</t>
+  </si>
+  <si>
+    <t>Magma jet</t>
+  </si>
+  <si>
+    <t>Fire Bettle</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Charge</t>
   </si>
 </sst>
 </file>
@@ -646,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1187,33 +1211,138 @@
         <v>73</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="7">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4">
+        <v>4</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="4">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2" t="s">
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="7">
-        <v>0</v>
-      </c>
-      <c r="H22" s="4">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2" t="s">
+      <c r="G23" s="7">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="K22" s="4">
-        <v>0</v>
-      </c>
-      <c r="L22" s="2" t="s">
+      <c r="K23" s="4">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="7">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>1</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K24" s="4">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" s="7">
+        <v>50</v>
+      </c>
+      <c r="H25" s="4">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K25" s="4">
+        <v>6</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>